<commit_message>
even more tests added to test dataset
</commit_message>
<xml_diff>
--- a/occurrence-processor/src/test/resources/dataset_to_test_gbif_interpretation.xlsx
+++ b/occurrence-processor/src/test/resources/dataset_to_test_gbif_interpretation.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1240" yWindow="1300" windowWidth="37320" windowHeight="17440" tabRatio="500"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="37080" windowHeight="22140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="maximumDepthInMeters" localSheetId="0">Sheet1!$AB$1</definedName>
-    <definedName name="maximumDistanceAboveSurfaceInMeters" localSheetId="0">Sheet1!$AD$1</definedName>
+    <definedName name="maximumDepthInMeters" localSheetId="0">Sheet1!$V$1</definedName>
+    <definedName name="maximumDistanceAboveSurfaceInMeters" localSheetId="0">Sheet1!#REF!</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="141">
   <si>
     <t>occurrenceID</t>
     <phoneticPr fontId="1"/>
@@ -33,22 +33,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>references</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>institutionCode</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>collectionCode</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>catalogNumber</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>basisOfRecord</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -104,14 +88,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>minimumDistanceAboveSurfaceInMeters</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>maximumDistanceAboveSurfaceInMeters</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>continent</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -432,6 +408,180 @@
   </si>
   <si>
     <t>Validate eventDate is contradicts the individual year, month, day</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Validate eventDate is created from the individual year, month, day. Expected eventDate= Apr 9, 1964</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Validate partial eventDate is created from the individual year and month. Expected eventDate= Apr, 1964</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1000ft</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>one hundred meters</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Validate non numeric depth supplied. Expected: no interpreted depth, issue = DEPTH_NON_NUMERIC</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Validate depth supplied in feet, is converted to meters. Expected: Depth = 304.8, issue = DEPTH_NOT_METRIC</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Validate elevation calcualted from max + min / 2. Expected: Elevation = 11</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Validate elevation above 17km is unlikely. Expected: Elevation = 17000 issue = ELEVATION_MIN_MAX_SWAPPED</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Validate depth calcualted from max + min / 2. Expected: Depth = 11</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Validate depth below 11,000m is unlikely. Expected: Elevation = 11000, issue = DEPTH_UNLIKELY</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Validate depth with negative value is unlikely. Expected: issue = DEPTH_UNLIKELY</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Validate elevation supplied in feet, is converted to meters. Expected: Elevation = 304.8, issue = ELEVATION_NOT_METRIC</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Validate elevation below Mariana Trench (-11,000m) is unlikely. Expected: issue = DEPTH_UNLIKELY</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Validate min depth is larger than max depth. issue = DEPTH_MIN_MAX_SWAPPED</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Validate min elevation is larger than max elevation. issue = ELEVATION_MIN_MAX_SWAPPED</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Validate non numeric elevation supplied. Expected: no interpreted elevation, issue = ELEVATION_NON_NUMERIC</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Oenante</t>
+  </si>
+  <si>
+    <t>kingdom</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Plantae</t>
+  </si>
+  <si>
+    <t>Kyle</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Validate the match to the taxonomic backbone was not perfect, but FUZZY. Expected: issue = TAXON_MATCH_FUZZY</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Validate the match to the taxonomic backbone can only be done on a higher rank and not the scientific name. Expected: issue = TAXON_MATCH_HIGHERRANK</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Validate Matching to the taxonomic backbone cannot be done cause there was no match at all. Expected: issue = TAXON_MATCH_NONE</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Braak</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Kyle</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Validate the typeStatus that doesn't match our ENUM. Expected: issue = TYPE_STATUS_INVALID</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Plastotype</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Validate the typeStatus that matches our ENUM. Expected: typeStatus = Plastotype</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Made up type</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Validate we can interpret coordinateAccuracy from only dwc:coordinatePrecision (direct copy). Expected: coodinateAccuracy = 1.5</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Validate the stateProvince containing a carriage return \r is cleaned. Expected: New Brunswick</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>New \r Brunswick</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Validate the waterBody containing a carriage return \r is cleaned. Expected: North Sea</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>North \r Sea</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Validate we can interpret coordinateAccuracy from dwc:coordinateUncertaintyInMeters. Expected: coodinateAccuracy = TODO calculation</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Validate we can interpret coordinateAccuracy from BOTH dwc:coordinatePrecision and coordinateUncertaintyInMeters. Expected: coodinateAccuracy = TODO calculation</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Validate BoR containing a carriage return \r is cleaned. Expected: PreservedSpecimen</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Preserved\rSpecimen</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Validate sex containing a carriage return \r is cleaned. Expected: Male</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Male \r</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Validate lifeStage containing a carriage return \r is cleaned. Expected: Adult</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Adult \r</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Validate establishmentMeans containing a carriage return \r is cleaned. Expected: Native</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Native \r</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -441,7 +591,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="0.0000_ "/>
-    <numFmt numFmtId="178" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="177" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -510,7 +660,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="120">
+  <cellStyleXfs count="236">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -631,8 +781,124 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -641,9 +907,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="120">
+  <cellStyles count="236">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -707,6 +976,64 @@
     <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="161" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="163" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="165" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="167" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="169" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="171" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="173" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="175" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="177" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="181" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="183" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="185" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="187" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="189" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="191" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="193" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="195" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="197" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="199" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="201" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="203" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="205" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="207" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="209" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="211" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="213" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="215" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="217" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="219" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="221" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="223" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="225" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="227" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="229" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="231" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="233" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="235" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
@@ -763,6 +1090,64 @@
     <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="146" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="150" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="152" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="154" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="156" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="158" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="160" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="162" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="164" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="166" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="168" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="170" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="172" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="174" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="176" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="178" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="180" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="182" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="184" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="186" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="188" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="190" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="192" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="194" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="196" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="198" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="200" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="202" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="204" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="206" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="208" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="210" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="212" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="214" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="216" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="218" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="220" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="222" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="224" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="226" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="228" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="230" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="232" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="234" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1092,131 +1477,126 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH46"/>
+  <dimension ref="A1:AC73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="23.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="135" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="151.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.1640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="30.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.83203125" style="6" customWidth="1"/>
-    <col min="19" max="19" width="16.33203125" style="6" customWidth="1"/>
-    <col min="20" max="20" width="11.1640625" style="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5" style="1" customWidth="1"/>
-    <col min="22" max="22" width="10.83203125" style="1"/>
-    <col min="23" max="23" width="19" style="1" customWidth="1"/>
-    <col min="24" max="24" width="28.83203125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="26" style="1" customWidth="1"/>
-    <col min="26" max="26" width="26.5" style="1" customWidth="1"/>
-    <col min="27" max="27" width="22.83203125" style="1" customWidth="1"/>
-    <col min="28" max="28" width="23.33203125" style="1" customWidth="1"/>
-    <col min="29" max="29" width="37.33203125" style="1" customWidth="1"/>
-    <col min="30" max="30" width="38.5" style="1" customWidth="1"/>
-    <col min="31" max="31" width="13.83203125" style="1" customWidth="1"/>
-    <col min="32" max="32" width="11.5" style="1" customWidth="1"/>
-    <col min="33" max="33" width="12" style="1" customWidth="1"/>
-    <col min="34" max="16384" width="10.83203125" style="1"/>
+    <col min="4" max="5" width="23.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="26.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="30.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.33203125" style="1" customWidth="1"/>
+    <col min="29" max="29" width="11.5" style="1" customWidth="1"/>
+    <col min="30" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:29">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="S1" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>17</v>
+      <c r="Z1" s="5" t="s">
+        <v>114</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>19</v>
@@ -1224,236 +1604,239 @@
       <c r="AC1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AD1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34">
+    </row>
+    <row r="2" spans="1:29">
       <c r="A2" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A2))</f>
+        <f t="shared" ref="A2:A66" si="0">CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A2))</f>
         <v>urn:lsid:gbif.org:Test:2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C2" s="8">
         <v>23078</v>
       </c>
-      <c r="Q2" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:34">
+      <c r="Y2" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29">
       <c r="A3" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A3))</f>
+        <f t="shared" si="0"/>
         <v>urn:lsid:gbif.org:Test:3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:34">
+        <v>27</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29">
       <c r="A4" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A4))</f>
+        <f t="shared" si="0"/>
         <v>urn:lsid:gbif.org:Test:4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q4" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:34">
+        <v>26</v>
+      </c>
+      <c r="Y4" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29">
       <c r="A5" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A5))</f>
+        <f t="shared" si="0"/>
         <v>urn:lsid:gbif.org:Test:5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C5" s="8">
         <v>44135</v>
       </c>
-    </row>
-    <row r="6" spans="1:34">
+      <c r="Y5" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29">
       <c r="A6" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A6))</f>
+        <f t="shared" si="0"/>
         <v>urn:lsid:gbif.org:Test:6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="7" spans="1:34">
+        <v>87</v>
+      </c>
+      <c r="Y6" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29">
       <c r="A7" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A7))</f>
+        <f t="shared" si="0"/>
         <v>urn:lsid:gbif.org:Test:7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D7" s="8">
         <v>23078</v>
       </c>
-      <c r="Q7" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:34">
+      <c r="Y7" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29">
       <c r="A8" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A8))</f>
+        <f t="shared" si="0"/>
         <v>urn:lsid:gbif.org:Test:8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q8" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:34">
+        <v>27</v>
+      </c>
+      <c r="Y8" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29">
       <c r="A9" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A9))</f>
+        <f t="shared" si="0"/>
         <v>urn:lsid:gbif.org:Test:9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q9" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:34">
+        <v>26</v>
+      </c>
+      <c r="Y9" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29">
       <c r="A10" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A10))</f>
+        <f t="shared" si="0"/>
         <v>urn:lsid:gbif.org:Test:10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D10" s="8">
         <v>44135</v>
       </c>
-    </row>
-    <row r="11" spans="1:34">
+      <c r="Y10" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29">
       <c r="A11" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A11))</f>
+        <f t="shared" si="0"/>
         <v>urn:lsid:gbif.org:Test:11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="12" spans="1:34">
+        <v>87</v>
+      </c>
+      <c r="Y11" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29">
       <c r="A12" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A12))</f>
+        <f t="shared" si="0"/>
         <v>urn:lsid:gbif.org:Test:12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E12" s="8">
         <v>23078</v>
       </c>
-      <c r="Q12" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:34">
+      <c r="Y12" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29">
       <c r="A13" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A13))</f>
+        <f t="shared" si="0"/>
         <v>urn:lsid:gbif.org:Test:13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q13" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:34">
+        <v>27</v>
+      </c>
+      <c r="Y13" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29">
       <c r="A14" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A14))</f>
+        <f t="shared" si="0"/>
         <v>urn:lsid:gbif.org:Test:14</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q14" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:34">
+        <v>26</v>
+      </c>
+      <c r="Y14" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29">
       <c r="A15" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A15))</f>
+        <f t="shared" si="0"/>
         <v>urn:lsid:gbif.org:Test:15</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E15" s="8">
         <v>44135</v>
       </c>
-    </row>
-    <row r="16" spans="1:34">
+      <c r="Y15" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29">
       <c r="A16" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A16))</f>
+        <f t="shared" si="0"/>
         <v>urn:lsid:gbif.org:Test:16</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19">
+        <v>87</v>
+      </c>
+      <c r="Y16" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25">
       <c r="A17" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A17))</f>
+        <f t="shared" si="0"/>
         <v>urn:lsid:gbif.org:Test:17</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="E17" s="8">
         <v>23078</v>
@@ -1467,498 +1850,944 @@
       <c r="H17" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="1:19">
+      <c r="Y17" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25">
       <c r="A18" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A18))</f>
+        <f t="shared" si="0"/>
         <v>urn:lsid:gbif.org:Test:18</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="L18" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="1">
+        <v>1964</v>
+      </c>
+      <c r="G18" s="1">
+        <v>4</v>
+      </c>
+      <c r="H18" s="1">
+        <v>9</v>
+      </c>
+      <c r="Y18" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25">
+      <c r="A19" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:19</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="1">
+        <v>1964</v>
+      </c>
+      <c r="G19" s="1">
+        <v>4</v>
+      </c>
+      <c r="Y19" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25">
+      <c r="A20" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:20</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y20" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25">
+      <c r="A21" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:21</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y21" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25">
+      <c r="A22" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:22</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y22" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25">
+      <c r="A23" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:23</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y23" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25">
+      <c r="A24" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:24</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25">
+      <c r="A25" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:25</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J25" s="1">
+        <v>25</v>
+      </c>
+      <c r="Y25" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25">
+      <c r="A26" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:26</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J26" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Q18" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19">
-      <c r="A19" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A19))</f>
-        <v>urn:lsid:gbif.org:Test:19</v>
-      </c>
-      <c r="B19" s="1" t="s">
+      <c r="Y26" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25">
+      <c r="A27" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:27</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L19" s="1" t="s">
+      <c r="K27" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="Q19" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19">
-      <c r="A20" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A20))</f>
-        <v>urn:lsid:gbif.org:Test:20</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="L20" s="1" t="s">
+      <c r="Y27" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25">
+      <c r="A28" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:28</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="Q20" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19">
-      <c r="A21" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A21))</f>
-        <v>urn:lsid:gbif.org:Test:21</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19">
-      <c r="A22" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A22))</f>
-        <v>urn:lsid:gbif.org:Test:22</v>
-      </c>
-      <c r="B22" s="1" t="s">
+      <c r="K28" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="M22" s="1">
-        <v>25</v>
-      </c>
-      <c r="Q22" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19">
-      <c r="A23" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A23))</f>
-        <v>urn:lsid:gbif.org:Test:23</v>
-      </c>
-      <c r="B23" s="1" t="s">
+      <c r="Y28" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25">
+      <c r="A29" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:29</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25">
+      <c r="A30" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:30</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="M23" s="1" t="s">
+      <c r="L30" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="Q23" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19">
-      <c r="A24" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A24))</f>
-        <v>urn:lsid:gbif.org:Test:24</v>
-      </c>
-      <c r="B24" s="1" t="s">
+      <c r="Y30" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25">
+      <c r="A31" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:31</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N24" s="1" t="s">
+      <c r="L31" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="Q24" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19">
-      <c r="A25" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A25))</f>
-        <v>urn:lsid:gbif.org:Test:25</v>
-      </c>
-      <c r="B25" s="1" t="s">
+      <c r="Y31" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25">
+      <c r="A32" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:32</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25">
+      <c r="A33" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:33</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="N25" s="1" t="s">
+      <c r="M33" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Q25" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19">
-      <c r="A26" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A26))</f>
-        <v>urn:lsid:gbif.org:Test:26</v>
-      </c>
-      <c r="B26" s="1" t="s">
+      <c r="Y33" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25">
+      <c r="A34" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:34</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="O26" s="1" t="s">
+      <c r="M34" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="Q26" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19">
-      <c r="A27" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A27))</f>
-        <v>urn:lsid:gbif.org:Test:27</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="O27" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q27" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19">
-      <c r="A28" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A28))</f>
-        <v>urn:lsid:gbif.org:Test:28</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="P28" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q28" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19">
-      <c r="A29" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A29))</f>
-        <v>urn:lsid:gbif.org:Test:29</v>
-      </c>
-      <c r="B29" s="1" t="s">
+      <c r="Y34" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25">
+      <c r="A35" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:35</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25">
+      <c r="A36" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:36</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="P29" s="1" t="s">
+      <c r="N36" s="6">
+        <v>-88.123400000000004</v>
+      </c>
+      <c r="O36" s="6">
+        <v>100</v>
+      </c>
+      <c r="Y36" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25">
+      <c r="A37" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:37</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N37" s="6">
+        <v>91</v>
+      </c>
+      <c r="O37" s="6">
+        <v>100</v>
+      </c>
+      <c r="Y37" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25">
+      <c r="A38" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:38</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="Q29" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19">
-      <c r="A30" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A30))</f>
-        <v>urn:lsid:gbif.org:Test:30</v>
-      </c>
-      <c r="B30" s="1" t="s">
+      <c r="N38" s="6">
+        <v>50</v>
+      </c>
+      <c r="O38" s="6">
+        <v>-178.1234</v>
+      </c>
+      <c r="Y38" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25">
+      <c r="A39" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:39</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N39" s="6">
+        <v>50</v>
+      </c>
+      <c r="O39" s="6">
+        <v>181</v>
+      </c>
+      <c r="Y39" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25">
+      <c r="A40" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:40</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="N40" s="6">
+        <v>12.568300000000001</v>
+      </c>
+      <c r="O40" s="6">
+        <v>55.676099999999998</v>
+      </c>
+      <c r="R40" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y40" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25">
+      <c r="A41" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:41</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="Q30" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="R30" s="6">
-        <v>-88.123400000000004</v>
-      </c>
-      <c r="S30" s="6">
+      <c r="N41" s="6">
+        <v>0</v>
+      </c>
+      <c r="O41" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y41" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25">
+      <c r="A42" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:42</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="N42" s="6">
+        <v>55.676099999999998</v>
+      </c>
+      <c r="O42" s="6">
+        <v>12.568300000000001</v>
+      </c>
+      <c r="R42" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y42" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25">
+      <c r="A43" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:43</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="N43" s="6">
+        <v>12.568300000000001</v>
+      </c>
+      <c r="O43" s="6">
+        <v>55.676099999999998</v>
+      </c>
+      <c r="P43" s="1">
+        <v>30</v>
+      </c>
+      <c r="Y43" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25">
+      <c r="A44" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:44</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="N44" s="6">
+        <v>12.568300000000001</v>
+      </c>
+      <c r="O44" s="6">
+        <v>55.676099999999998</v>
+      </c>
+      <c r="Q44" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="Y44" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25">
+      <c r="A45" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:45</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="N45" s="6">
+        <v>12.568300000000001</v>
+      </c>
+      <c r="O45" s="6">
+        <v>55.676099999999998</v>
+      </c>
+      <c r="P45" s="1">
+        <v>30</v>
+      </c>
+      <c r="Q45" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25">
+      <c r="A46" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:46</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N46" s="6">
+        <v>55.676099999999998</v>
+      </c>
+      <c r="O46" s="6">
+        <v>12.568300000000001</v>
+      </c>
+      <c r="R46" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S46" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y46" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25">
+      <c r="A47" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:47</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R47" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y47" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25">
+      <c r="A48" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:48</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="N48" s="6">
+        <v>55.676099999999998</v>
+      </c>
+      <c r="O48" s="6">
+        <v>12.568300000000001</v>
+      </c>
+      <c r="Y48" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:25">
+      <c r="A49" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:49</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R49" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="S49" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="T49" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y49" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="50" spans="1:25">
+      <c r="A50" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:50</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="T50" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y50" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="51" spans="1:25">
+      <c r="A51" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:51</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="T51" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y51" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="1:25">
+      <c r="A52" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:52</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="N52" s="6">
+        <v>55.676099999999998</v>
+      </c>
+      <c r="O52" s="6">
+        <v>12.568300000000001</v>
+      </c>
+      <c r="Y52" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="53" spans="1:25">
+      <c r="A53" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:53</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="N53" s="7">
+        <v>-55.676099999999998</v>
+      </c>
+      <c r="O53" s="7">
+        <v>12.568300000000001</v>
+      </c>
+      <c r="R53" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S53" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="T53" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y53" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="54" spans="1:25">
+      <c r="A54" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:54</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N54" s="7">
+        <v>55.676099999999998</v>
+      </c>
+      <c r="O54" s="7">
+        <v>-12.568300000000001</v>
+      </c>
+      <c r="R54" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S54" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="T54" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y54" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="55" spans="1:25">
+      <c r="A55" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:55</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="U55" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y55" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="56" spans="1:25">
+      <c r="A56" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:56</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="U56" s="1">
+        <v>10</v>
+      </c>
+      <c r="V56" s="1">
+        <v>12</v>
+      </c>
+      <c r="Y56" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="57" spans="1:25">
+      <c r="A57" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:57</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="U57" s="1">
+        <v>12000</v>
+      </c>
+      <c r="Y57" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="58" spans="1:25">
+      <c r="A58" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:58</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="U58" s="1">
+        <v>-1000</v>
+      </c>
+      <c r="Y58" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="59" spans="1:25">
+      <c r="A59" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:59</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="U59" s="1">
+        <v>12</v>
+      </c>
+      <c r="V59" s="1">
+        <v>10</v>
+      </c>
+      <c r="Y59" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="60" spans="1:25">
+      <c r="A60" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:60</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="U60" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="31" spans="1:19">
-      <c r="A31" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A31))</f>
-        <v>urn:lsid:gbif.org:Test:31</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q31" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="R31" s="6">
-        <v>91</v>
-      </c>
-      <c r="S31" s="6">
+      <c r="Y60" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="61" spans="1:25">
+      <c r="A61" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:61</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="W61" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y61" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="62" spans="1:25">
+      <c r="A62" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:62</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="W62" s="1">
+        <v>10</v>
+      </c>
+      <c r="X62" s="1">
+        <v>12</v>
+      </c>
+      <c r="Y62" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="63" spans="1:25">
+      <c r="A63" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:63</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="W63" s="1">
+        <v>17000</v>
+      </c>
+      <c r="Y63" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="64" spans="1:25">
+      <c r="A64" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:64</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="W64" s="1">
+        <v>-1000</v>
+      </c>
+      <c r="Y64" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="65" spans="1:29">
+      <c r="A65" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:65</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="W65" s="1">
+        <v>12</v>
+      </c>
+      <c r="X65" s="1">
+        <v>10</v>
+      </c>
+      <c r="Y65" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="66" spans="1:29">
+      <c r="A66" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:lsid:gbif.org:Test:66</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="W66" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="32" spans="1:19">
-      <c r="A32" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A32))</f>
-        <v>urn:lsid:gbif.org:Test:32</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q32" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="R32" s="6">
-        <v>50</v>
-      </c>
-      <c r="S32" s="6">
-        <v>-178.1234</v>
-      </c>
-    </row>
-    <row r="33" spans="1:22">
-      <c r="A33" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A33))</f>
-        <v>urn:lsid:gbif.org:Test:33</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q33" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="R33" s="6">
-        <v>50</v>
-      </c>
-      <c r="S33" s="6">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="34" spans="1:22">
-      <c r="A34" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A34))</f>
-        <v>urn:lsid:gbif.org:Test:34</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q34" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="R34" s="6">
-        <v>12.568300000000001</v>
-      </c>
-      <c r="S34" s="6">
-        <v>55.676099999999998</v>
-      </c>
-      <c r="T34" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="35" spans="1:22">
-      <c r="A35" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A35))</f>
-        <v>urn:lsid:gbif.org:Test:35</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q35" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="R35" s="6">
-        <v>0</v>
-      </c>
-      <c r="S35" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:22">
-      <c r="A36" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A36))</f>
-        <v>urn:lsid:gbif.org:Test:36</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q36" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="R36" s="6">
-        <v>55.676099999999998</v>
-      </c>
-      <c r="S36" s="6">
-        <v>12.568300000000001</v>
-      </c>
-      <c r="T36" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="37" spans="1:22">
-      <c r="A37" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A37))</f>
-        <v>urn:lsid:gbif.org:Test:37</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q37" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="R37" s="6">
-        <v>55.676099999999998</v>
-      </c>
-      <c r="S37" s="6">
-        <v>12.568300000000001</v>
-      </c>
-      <c r="T37" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="U37" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="38" spans="1:22">
-      <c r="A38" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A38))</f>
-        <v>urn:lsid:gbif.org:Test:38</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q38" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="T38" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="39" spans="1:22">
-      <c r="A39" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A39))</f>
-        <v>urn:lsid:gbif.org:Test:39</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q39" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="R39" s="6">
-        <v>55.676099999999998</v>
-      </c>
-      <c r="S39" s="6">
-        <v>12.568300000000001</v>
-      </c>
-    </row>
-    <row r="40" spans="1:22">
-      <c r="A40" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A40))</f>
-        <v>urn:lsid:gbif.org:Test:40</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q40" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="T40" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="U40" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="V40" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="41" spans="1:22">
-      <c r="A41" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A41))</f>
-        <v>urn:lsid:gbif.org:Test:41</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q41" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="V41" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="42" spans="1:22">
-      <c r="A42" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A42))</f>
-        <v>urn:lsid:gbif.org:Test:42</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q42" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="V42" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="43" spans="1:22">
-      <c r="A43" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A43))</f>
-        <v>urn:lsid:gbif.org:Test:43</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q43" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="R43" s="6">
-        <v>55.676099999999998</v>
-      </c>
-      <c r="S43" s="6">
-        <v>12.568300000000001</v>
-      </c>
-    </row>
-    <row r="44" spans="1:22">
-      <c r="A44" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A44))</f>
-        <v>urn:lsid:gbif.org:Test:44</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q44" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="R44" s="7">
-        <v>-55.676099999999998</v>
-      </c>
-      <c r="S44" s="7">
-        <v>12.568300000000001</v>
-      </c>
-      <c r="T44" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="U44" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="V44" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="45" spans="1:22">
-      <c r="A45" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A45))</f>
-        <v>urn:lsid:gbif.org:Test:45</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q45" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="R45" s="7">
-        <v>55.676099999999998</v>
-      </c>
-      <c r="S45" s="7">
-        <v>-12.568300000000001</v>
-      </c>
-      <c r="T45" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="U45" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="V45" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="46" spans="1:22">
-      <c r="A46" s="4"/>
+      <c r="Y66" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="67" spans="1:29">
+      <c r="A67" s="4" t="str">
+        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A67))</f>
+        <v>urn:lsid:gbif.org:Test:67</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y67" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z67" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="68" spans="1:29">
+      <c r="A68" s="4" t="str">
+        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A68))</f>
+        <v>urn:lsid:gbif.org:Test:68</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="Y68" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z68" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="69" spans="1:29">
+      <c r="A69" s="4" t="str">
+        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A69))</f>
+        <v>urn:lsid:gbif.org:Test:69</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y69" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z69" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="70" spans="1:29">
+      <c r="A70" s="4" t="str">
+        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A70))</f>
+        <v>urn:lsid:gbif.org:Test:70</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="Y70" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA70" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="71" spans="1:29">
+      <c r="A71" s="4" t="str">
+        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A71))</f>
+        <v>urn:lsid:gbif.org:Test:71</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="Y71" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA71" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="72" spans="1:29">
+      <c r="A72" s="4" t="str">
+        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A72))</f>
+        <v>urn:lsid:gbif.org:Test:72</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AB72" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="73" spans="1:29">
+      <c r="A73" s="4" t="str">
+        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A73))</f>
+        <v>urn:lsid:gbif.org:Test:73</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="AC73" s="1" t="s">
+        <v>130</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
another couple test records added to test dataset
</commit_message>
<xml_diff>
--- a/occurrence-processor/src/test/resources/dataset_to_test_gbif_interpretation.xlsx
+++ b/occurrence-processor/src/test/resources/dataset_to_test_gbif_interpretation.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="143">
   <si>
     <t>occurrenceID</t>
     <phoneticPr fontId="1"/>
@@ -582,6 +582,14 @@
   </si>
   <si>
     <t>Native \r</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Validate depthAccuracy calculated correctly from (max - min) / 2. Expected: depthAccuracy = 1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Validate elevationAccuracy calculated correctly from (max - min) / 2. Expected: elevationAccuracy = 1</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -660,7 +668,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="236">
+  <cellStyleXfs count="246">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -668,6 +676,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -912,7 +930,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="236">
+  <cellStyles count="246">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -1034,6 +1052,11 @@
     <cellStyle name="Followed Hyperlink" xfId="231" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="233" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="235" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="237" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="239" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="241" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="243" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="245" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
@@ -1148,6 +1171,11 @@
     <cellStyle name="Hyperlink" xfId="230" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="232" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="234" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="236" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="238" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="240" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="242" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="244" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1477,10 +1505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC73"/>
+  <dimension ref="A1:AC75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1607,7 +1635,7 @@
     </row>
     <row r="2" spans="1:29">
       <c r="A2" s="4" t="str">
-        <f t="shared" ref="A2:A66" si="0">CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A2))</f>
+        <f t="shared" ref="A2:A68" si="0">CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A2))</f>
         <v>urn:lsid:gbif.org:Test:2</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2600,10 +2628,13 @@
         <v>urn:lsid:gbif.org:Test:61</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="W61" s="1" t="s">
-        <v>99</v>
+        <v>141</v>
+      </c>
+      <c r="U61" s="1">
+        <v>12</v>
+      </c>
+      <c r="V61" s="1">
+        <v>10</v>
       </c>
       <c r="Y61" s="5" t="s">
         <v>31</v>
@@ -2615,13 +2646,10 @@
         <v>urn:lsid:gbif.org:Test:62</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="W62" s="1">
-        <v>10</v>
-      </c>
-      <c r="X62" s="1">
-        <v>12</v>
+        <v>108</v>
+      </c>
+      <c r="W62" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="Y62" s="5" t="s">
         <v>31</v>
@@ -2633,10 +2661,13 @@
         <v>urn:lsid:gbif.org:Test:63</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="W63" s="1">
-        <v>17000</v>
+        <v>10</v>
+      </c>
+      <c r="X63" s="1">
+        <v>12</v>
       </c>
       <c r="Y63" s="5" t="s">
         <v>31</v>
@@ -2648,10 +2679,10 @@
         <v>urn:lsid:gbif.org:Test:64</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="W64" s="1">
-        <v>-1000</v>
+        <v>17000</v>
       </c>
       <c r="Y64" s="5" t="s">
         <v>31</v>
@@ -2663,13 +2694,10 @@
         <v>urn:lsid:gbif.org:Test:65</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="W65" s="1">
-        <v>12</v>
-      </c>
-      <c r="X65" s="1">
-        <v>10</v>
+        <v>-1000</v>
       </c>
       <c r="Y65" s="5" t="s">
         <v>31</v>
@@ -2681,10 +2709,13 @@
         <v>urn:lsid:gbif.org:Test:66</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="W66" s="1" t="s">
-        <v>100</v>
+        <v>111</v>
+      </c>
+      <c r="W66" s="1">
+        <v>12</v>
+      </c>
+      <c r="X66" s="1">
+        <v>10</v>
       </c>
       <c r="Y66" s="5" t="s">
         <v>31</v>
@@ -2692,100 +2723,133 @@
     </row>
     <row r="67" spans="1:29">
       <c r="A67" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A67))</f>
+        <f t="shared" si="0"/>
         <v>urn:lsid:gbif.org:Test:67</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
+      </c>
+      <c r="W67" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="Y67" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="Z67" s="5" t="s">
-        <v>115</v>
+        <v>31</v>
       </c>
     </row>
     <row r="68" spans="1:29">
       <c r="A68" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A68))</f>
+        <f t="shared" si="0"/>
         <v>urn:lsid:gbif.org:Test:68</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>118</v>
+        <v>142</v>
+      </c>
+      <c r="W68" s="1">
+        <v>12</v>
+      </c>
+      <c r="X68" s="1">
+        <v>10</v>
       </c>
       <c r="Y68" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="Z68" s="5" t="s">
-        <v>116</v>
+        <v>31</v>
       </c>
     </row>
     <row r="69" spans="1:29">
       <c r="A69" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A69))</f>
+        <f t="shared" ref="A69:A75" si="1">CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A69))</f>
         <v>urn:lsid:gbif.org:Test:69</v>
       </c>
-      <c r="B69" s="9" t="s">
-        <v>119</v>
+      <c r="B69" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="Y69" s="5" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="Z69" s="5" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="70" spans="1:29">
       <c r="A70" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A70))</f>
+        <f t="shared" si="1"/>
         <v>urn:lsid:gbif.org:Test:70</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="Y70" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="AA70" s="1" t="s">
-        <v>123</v>
+        <v>113</v>
+      </c>
+      <c r="Z70" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="71" spans="1:29">
       <c r="A71" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A71))</f>
+        <f t="shared" si="1"/>
         <v>urn:lsid:gbif.org:Test:71</v>
       </c>
-      <c r="B71" s="1" t="s">
-        <v>122</v>
+      <c r="B71" s="9" t="s">
+        <v>119</v>
       </c>
       <c r="Y71" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="AA71" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
+      </c>
+      <c r="Z71" s="5" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="72" spans="1:29">
       <c r="A72" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A72))</f>
+        <f t="shared" si="1"/>
         <v>urn:lsid:gbif.org:Test:72</v>
       </c>
-      <c r="B72" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="AB72" s="1" t="s">
-        <v>128</v>
+      <c r="B72" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="Y72" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA72" s="1" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="73" spans="1:29">
       <c r="A73" s="4" t="str">
-        <f>CONCATENATE("urn:lsid:gbif.org:Test:", ROW(A73))</f>
+        <f t="shared" si="1"/>
         <v>urn:lsid:gbif.org:Test:73</v>
       </c>
       <c r="B73" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="Y73" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA73" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="74" spans="1:29">
+      <c r="A74" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>urn:lsid:gbif.org:Test:74</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AB74" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="75" spans="1:29">
+      <c r="A75" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>urn:lsid:gbif.org:Test:75</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="AC73" s="1" t="s">
+      <c r="AC75" s="1" t="s">
         <v>130</v>
       </c>
     </row>

</xml_diff>